<commit_message>
v1.1 - Added Processor selection support
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5C27B7E2-FA07-47C2-A449-838C3DD2E196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6B33A151-C632-4B54-B145-99217E5BF87E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="20745" windowHeight="13905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="20744" windowHeight="13904" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="remove" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>SearchString</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>₹50000</t>
+  </si>
+  <si>
+    <t>Processor</t>
+  </si>
+  <si>
+    <t>Snapdragon</t>
+  </si>
+  <si>
+    <t>Exynos</t>
   </si>
 </sst>
 </file>
@@ -449,15 +458,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54B1509-91DB-4B9E-B75F-BA8AD48CC7AA}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,8 +482,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -490,8 +502,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -506,6 +521,9 @@
       </c>
       <c r="E3" t="s">
         <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>